<commit_message>
Paper v2 dan Buku
</commit_message>
<xml_diff>
--- a/Laporan/BAHAN BUKU/Real Life Test/Percobaan CHP 172.xlsx
+++ b/Laporan/BAHAN BUKU/Real Life Test/Percobaan CHP 172.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>Badan</t>
   </si>
@@ -112,14 +112,25 @@
   </si>
   <si>
     <t>statis jadi dinamis</t>
+  </si>
+  <si>
+    <t>Akurasi (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -180,16 +191,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -201,10 +227,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -216,70 +242,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -356,19 +322,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -427,6 +380,43 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -434,6 +424,73 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -447,40 +504,16 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -491,39 +524,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -533,33 +587,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -840,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,169 +892,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="26" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="28"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="23"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="M2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="20" t="s">
+      <c r="O2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="20" t="s">
+      <c r="P2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="Q2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="20" t="s">
+      <c r="R2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="S2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="T2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="20" t="s">
+      <c r="U2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
         <v>4</v>
       </c>
-      <c r="D3" s="8">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8">
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
         <v>1</v>
       </c>
-      <c r="H3" s="8">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0</v>
-      </c>
-      <c r="L3" s="8">
-        <v>0</v>
-      </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-      <c r="N3" s="8">
-        <v>0</v>
-      </c>
-      <c r="O3" s="8">
-        <v>0</v>
-      </c>
-      <c r="P3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8">
-        <v>0</v>
-      </c>
-      <c r="R3" s="8">
-        <v>0</v>
-      </c>
-      <c r="S3" s="8">
-        <v>0</v>
-      </c>
-      <c r="T3" s="8">
-        <v>0</v>
-      </c>
-      <c r="U3" s="8">
-        <v>0</v>
-      </c>
-      <c r="V3" s="9">
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>0</v>
+      </c>
+      <c r="R3" s="6">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6">
+        <v>0</v>
+      </c>
+      <c r="T3" s="6">
+        <v>0</v>
+      </c>
+      <c r="U3" s="6">
+        <v>0</v>
+      </c>
+      <c r="V3" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="17" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>0</v>
       </c>
       <c r="D4" s="1">
@@ -1076,11 +1116,11 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="17" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>0</v>
       </c>
       <c r="D5" s="2">
@@ -1142,11 +1182,11 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>0</v>
       </c>
       <c r="D6" s="2">
@@ -1208,11 +1248,11 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>1</v>
       </c>
       <c r="D7" s="2">
@@ -1274,11 +1314,11 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>0</v>
       </c>
       <c r="D8" s="2">
@@ -1340,11 +1380,11 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <v>0</v>
       </c>
       <c r="D9" s="2">
@@ -1406,11 +1446,11 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="8">
         <v>0</v>
       </c>
       <c r="D10" s="2">
@@ -1472,14 +1512,14 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="20"/>
+      <c r="B11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10">
-        <v>0</v>
-      </c>
-      <c r="D11" s="22">
+      <c r="C11" s="8">
+        <v>0</v>
+      </c>
+      <c r="D11" s="18">
         <v>0</v>
       </c>
       <c r="E11" s="2">
@@ -1538,11 +1578,11 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="17" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="8">
         <v>0</v>
       </c>
       <c r="D12" s="2">
@@ -1604,11 +1644,11 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="8">
         <v>0</v>
       </c>
       <c r="D13" s="2">
@@ -1670,11 +1710,11 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <v>0</v>
       </c>
       <c r="D14" s="2">
@@ -1736,11 +1776,11 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="8">
         <v>0</v>
       </c>
       <c r="D15" s="2">
@@ -1802,11 +1842,11 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="8">
         <v>0</v>
       </c>
       <c r="D16" s="2">
@@ -1868,11 +1908,11 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="8">
         <v>0</v>
       </c>
       <c r="D17" s="2">
@@ -1934,11 +1974,11 @@
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <v>0</v>
       </c>
       <c r="D18" s="2">
@@ -2000,11 +2040,11 @@
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="17" t="s">
+      <c r="A19" s="20"/>
+      <c r="B19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <v>0</v>
       </c>
       <c r="D19" s="2">
@@ -2066,11 +2106,11 @@
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="17" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="8">
         <v>0</v>
       </c>
       <c r="D20" s="2">
@@ -2132,11 +2172,11 @@
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="17" t="s">
+      <c r="A21" s="20"/>
+      <c r="B21" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="8">
         <v>0</v>
       </c>
       <c r="D21" s="2">
@@ -2198,73 +2238,139 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25"/>
-      <c r="B22" s="18" t="s">
+      <c r="A22" s="20"/>
+      <c r="B22" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="11">
-        <v>0</v>
-      </c>
-      <c r="D22" s="4">
-        <v>0</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0</v>
-      </c>
-      <c r="F22" s="4">
-        <v>0</v>
-      </c>
-      <c r="G22" s="4">
-        <v>0</v>
-      </c>
-      <c r="H22" s="4">
-        <v>0</v>
-      </c>
-      <c r="I22" s="4">
-        <v>0</v>
-      </c>
-      <c r="J22" s="4">
-        <v>0</v>
-      </c>
-      <c r="K22" s="4">
-        <v>0</v>
-      </c>
-      <c r="L22" s="4">
-        <v>0</v>
-      </c>
-      <c r="M22" s="4">
-        <v>0</v>
-      </c>
-      <c r="N22" s="4">
-        <v>0</v>
-      </c>
-      <c r="O22" s="4">
-        <v>0</v>
-      </c>
-      <c r="P22" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="4">
-        <v>0</v>
-      </c>
-      <c r="R22" s="4">
-        <v>0</v>
-      </c>
-      <c r="S22" s="4">
-        <v>0</v>
-      </c>
-      <c r="T22" s="4">
+      <c r="C22" s="25">
+        <v>0</v>
+      </c>
+      <c r="D22" s="26">
+        <v>0</v>
+      </c>
+      <c r="E22" s="26">
+        <v>0</v>
+      </c>
+      <c r="F22" s="26">
+        <v>0</v>
+      </c>
+      <c r="G22" s="26">
+        <v>0</v>
+      </c>
+      <c r="H22" s="26">
+        <v>0</v>
+      </c>
+      <c r="I22" s="26">
+        <v>0</v>
+      </c>
+      <c r="J22" s="26">
+        <v>0</v>
+      </c>
+      <c r="K22" s="26">
+        <v>0</v>
+      </c>
+      <c r="L22" s="26">
+        <v>0</v>
+      </c>
+      <c r="M22" s="26">
+        <v>0</v>
+      </c>
+      <c r="N22" s="26">
+        <v>0</v>
+      </c>
+      <c r="O22" s="26">
+        <v>0</v>
+      </c>
+      <c r="P22" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="26">
+        <v>0</v>
+      </c>
+      <c r="R22" s="26">
+        <v>0</v>
+      </c>
+      <c r="S22" s="26">
+        <v>0</v>
+      </c>
+      <c r="T22" s="26">
         <v>2</v>
       </c>
-      <c r="U22" s="4">
-        <v>0</v>
-      </c>
-      <c r="V22" s="5">
+      <c r="U22" s="26">
+        <v>0</v>
+      </c>
+      <c r="V22" s="27">
         <v>3</v>
       </c>
     </row>
+    <row r="23" spans="1:22" s="33" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30">
+        <v>80</v>
+      </c>
+      <c r="D23" s="31">
+        <v>100</v>
+      </c>
+      <c r="E23" s="31">
+        <v>60</v>
+      </c>
+      <c r="F23" s="31">
+        <v>60</v>
+      </c>
+      <c r="G23" s="31">
+        <v>80</v>
+      </c>
+      <c r="H23" s="31">
+        <v>80</v>
+      </c>
+      <c r="I23" s="31">
+        <v>100</v>
+      </c>
+      <c r="J23" s="31">
+        <v>100</v>
+      </c>
+      <c r="K23" s="31">
+        <v>100</v>
+      </c>
+      <c r="L23" s="31">
+        <v>60</v>
+      </c>
+      <c r="M23" s="31">
+        <v>40</v>
+      </c>
+      <c r="N23" s="31">
+        <v>80</v>
+      </c>
+      <c r="O23" s="31">
+        <v>80</v>
+      </c>
+      <c r="P23" s="31">
+        <v>100</v>
+      </c>
+      <c r="Q23" s="31">
+        <v>100</v>
+      </c>
+      <c r="R23" s="31">
+        <v>100</v>
+      </c>
+      <c r="S23" s="31">
+        <v>80</v>
+      </c>
+      <c r="T23" s="31">
+        <v>100</v>
+      </c>
+      <c r="U23" s="31">
+        <v>60</v>
+      </c>
+      <c r="V23" s="32">
+        <v>60</v>
+      </c>
+    </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D25">
@@ -2293,7 +2399,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D26">
@@ -2349,10 +2455,20 @@
         <v>24</v>
       </c>
     </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f>SUM(C23:V23)/20</f>
+        <v>81</v>
+      </c>
+      <c r="E29" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A3:A22"/>
     <mergeCell ref="C1:V1"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>